<commit_message>
added lots of local changes
</commit_message>
<xml_diff>
--- a/layouts/lightplay2a/lightplay2a-BillOfMaterials-screamingCircuits.xlsx
+++ b/layouts/lightplay2a/lightplay2a-BillOfMaterials-screamingCircuits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32040" windowHeight="19300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="153">
   <si>
     <t>10 uH inductor</t>
   </si>
@@ -42,9 +42,6 @@
     <t>LED Driver</t>
   </si>
   <si>
-    <t>Polarization Notes</t>
-  </si>
-  <si>
     <t>LT1615</t>
   </si>
   <si>
@@ -346,9 +343,6 @@
   </si>
   <si>
     <t>C9</t>
-  </si>
-  <si>
-    <t>C3-C6</t>
   </si>
   <si>
     <t>Item #</t>
@@ -447,6 +441,48 @@
   </si>
   <si>
     <t>PRT-08084</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Notes</t>
+  </si>
+  <si>
+    <t>C3,C5</t>
+  </si>
+  <si>
+    <t>C4,C6</t>
+  </si>
+  <si>
+    <t>on solder side</t>
+  </si>
+  <si>
+    <t>A4/A5</t>
+  </si>
+  <si>
+    <t>2 position male header (1/18 of 36 pin header)</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Light Play</t>
+  </si>
+  <si>
+    <t>Rev.</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Robbie Berg</t>
+  </si>
+  <si>
+    <t>Wellesley College</t>
+  </si>
+  <si>
+    <t>781-248-2404</t>
   </si>
 </sst>
 </file>
@@ -518,7 +554,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,12 +564,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,7 +648,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="269">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -888,8 +918,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -943,7 +979,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -959,8 +994,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="269">
+  <cellStyles count="275">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1116,6 +1160,9 @@
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
@@ -1229,6 +1276,9 @@
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1561,10 +1611,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1584,37 +1634,37 @@
   <sheetData>
     <row r="1" spans="1:12" s="12" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>113</v>
-      </c>
       <c r="K1" s="11" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="L1" s="11"/>
     </row>
@@ -1626,28 +1676,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2">
         <v>744025100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1661,25 +1711,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1690,16 +1740,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>4</v>
@@ -1708,10 +1758,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1722,61 +1772,62 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14" customHeight="1">
-      <c r="A6" s="1">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="16">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="J6" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1">
@@ -1786,52 +1837,52 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="28" customFormat="1">
+      <c r="A8" s="25">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="29" customFormat="1">
-      <c r="A8" s="26">
-        <v>7</v>
-      </c>
-      <c r="B8" s="27">
-        <v>1</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="K8" s="26"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
@@ -1841,28 +1892,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1873,28 +1924,28 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="H10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1905,28 +1956,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1937,25 +1988,25 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1966,28 +2017,28 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1998,28 +2049,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="30" customFormat="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="29" customFormat="1">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -2027,28 +2078,28 @@
         <v>1</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K15" s="15"/>
     </row>
-    <row r="16" spans="1:12" s="30" customFormat="1">
+    <row r="16" spans="1:12" s="29" customFormat="1">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -2056,28 +2107,28 @@
         <v>12</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>90</v>
-      </c>
       <c r="I16" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K16" s="15"/>
     </row>
@@ -2089,28 +2140,28 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2121,28 +2172,28 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="J18" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2153,28 +2204,28 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2185,28 +2236,28 @@
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="I20" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2217,28 +2268,28 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2249,28 +2300,28 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2278,129 +2329,132 @@
         <v>22</v>
       </c>
       <c r="B23" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16">
+        <v>2</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="13">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="H25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="29" customFormat="1">
+      <c r="A26" s="15">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16">
+        <v>1</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="25">
-        <v>23</v>
-      </c>
-      <c r="B24" s="13">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="F26" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="30" customFormat="1">
-      <c r="A25" s="15">
-        <v>24</v>
-      </c>
-      <c r="B25" s="16">
-        <v>1</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="13">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="J26" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1">
@@ -2410,59 +2464,106 @@
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>86</v>
+        <v>38</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:11" ht="16" thickBot="1">
-      <c r="B29" s="13"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" s="32"/>
-      <c r="I30"/>
-      <c r="J30"/>
+      <c r="J28" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="15">
+        <v>28</v>
+      </c>
+      <c r="B29" s="32">
+        <v>1</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="1:11" ht="16" thickBot="1">
+      <c r="B30" s="13"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H31" s="22">
-        <v>22</v>
-      </c>
+      <c r="G31" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" s="31"/>
       <c r="I31"/>
       <c r="J31"/>
     </row>
@@ -2472,10 +2573,10 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H32" s="22">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -2486,41 +2587,49 @@
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33" s="21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H33" s="22">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="3:10" ht="16" thickBot="1">
+    <row r="34" spans="3:10">
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34"/>
-      <c r="G34" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="H34" s="24" t="s">
-        <v>130</v>
+      <c r="G34" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H34" s="22">
+        <v>6</v>
       </c>
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="3:10">
+    <row r="35" spans="3:10" ht="16" thickBot="1">
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
       <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
+      <c r="G35" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>128</v>
+      </c>
       <c r="I35"/>
       <c r="J35"/>
     </row>
     <row r="36" spans="3:10">
-      <c r="C36"/>
-      <c r="D36"/>
+      <c r="C36" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36"/>
@@ -2529,8 +2638,12 @@
       <c r="J36"/>
     </row>
     <row r="37" spans="3:10">
-      <c r="C37"/>
-      <c r="D37"/>
+      <c r="C37" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>148</v>
+      </c>
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
@@ -2539,8 +2652,12 @@
       <c r="J37"/>
     </row>
     <row r="38" spans="3:10">
-      <c r="C38"/>
-      <c r="D38"/>
+      <c r="C38" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" t="s">
+        <v>150</v>
+      </c>
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38"/>
@@ -2550,7 +2667,9 @@
     </row>
     <row r="39" spans="3:10">
       <c r="C39"/>
-      <c r="D39"/>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
       <c r="E39"/>
       <c r="F39"/>
       <c r="G39"/>
@@ -2560,7 +2679,9 @@
     </row>
     <row r="40" spans="3:10">
       <c r="C40"/>
-      <c r="D40"/>
+      <c r="D40" t="s">
+        <v>152</v>
+      </c>
       <c r="E40"/>
       <c r="F40"/>
       <c r="G40"/>
@@ -2668,13 +2789,23 @@
       <c r="I50"/>
       <c r="J50"/>
     </row>
+    <row r="51" spans="3:10">
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="51" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="44" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>